<commit_message>
#SSW-620 Import Excel angepasst
</commit_message>
<xml_diff>
--- a/Common/Style/Resource/Template/Fakturierung Import.xlsx
+++ b/Common/Style/Resource/Template/Fakturierung Import.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rackel\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730"/>
   </bookViews>
@@ -24,19 +29,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
-    <t>Verursacher Vorname</t>
-  </si>
-  <si>
-    <t>Verursacher Nachname</t>
-  </si>
-  <si>
     <t>Beitragsart</t>
-  </si>
-  <si>
-    <t>Zahler Vorname</t>
-  </si>
-  <si>
-    <t>Zahler Nachname</t>
   </si>
   <si>
     <t>Debitorennummer</t>
@@ -64,15 +57,6 @@
     <t>Essensgeld</t>
   </si>
   <si>
-    <t>DE00 0000 0000 0000 0000 00</t>
-  </si>
-  <si>
-    <t>DE11 1111 1111 1111 1111 11</t>
-  </si>
-  <si>
-    <t>*Varianten müssen heißen wie in der Schulsoftware</t>
-  </si>
-  <si>
     <t>*forlaufend</t>
   </si>
   <si>
@@ -88,23 +72,13 @@
     <t>Zählung</t>
   </si>
   <si>
-    <t>Verursacher Geburtstag</t>
-  </si>
-  <si>
     <t>Individueller Preis</t>
   </si>
   <si>
-    <t>Mandatsreferenznummer gültig ab</t>
-  </si>
-  <si>
     <t>Bank Name</t>
   </si>
   <si>
     <t>Kontoinhaber</t>
-  </si>
-  <si>
-    <t>*Exisiteren die Varianten in der Schulsoftware nicht,
- ist es ein individueller Preis und damit eine Pflichteingabe</t>
   </si>
   <si>
     <t>*Ab wann soll die Zahlung nicht mehr gezogen werden</t>
@@ -129,9 +103,6 @@
     <t>Klaus</t>
   </si>
   <si>
-    <t>Klaus Mustermann</t>
-  </si>
-  <si>
     <t>Hort 1. Kind</t>
   </si>
   <si>
@@ -141,9 +112,6 @@
     <t>Monika</t>
   </si>
   <si>
-    <t>Monika Mustermann</t>
-  </si>
-  <si>
     <t>…</t>
   </si>
   <si>
@@ -154,12 +122,50 @@
   </si>
   <si>
     <t>FEOOTA2L852</t>
+  </si>
+  <si>
+    <t>DE00000000000000000000</t>
+  </si>
+  <si>
+    <t>DE11111111111111111111</t>
+  </si>
+  <si>
+    <t>Mustermann Klaus</t>
+  </si>
+  <si>
+    <t>Mustermann Monika</t>
+  </si>
+  <si>
+    <t>*Exisiteren die Preis-Variante nicht,
+wird der Individuelle Preis zur Pflichteingabe</t>
+  </si>
+  <si>
+    <t>*Preis-Varianten müssen heißen
+wie in der Schulsoftware</t>
+  </si>
+  <si>
+    <t>Beitragsverursacher Vorname</t>
+  </si>
+  <si>
+    <t>Beitragsverursacher Nachname</t>
+  </si>
+  <si>
+    <t>Beitragsverursacher Geburtstag</t>
+  </si>
+  <si>
+    <t>Mandatsreferenznummer gültig ab</t>
+  </si>
+  <si>
+    <t>Beitragszahler Vorname</t>
+  </si>
+  <si>
+    <t>Beitragszahler Nachname</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ _€"/>
   </numFmts>
@@ -212,12 +218,7 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -233,12 +234,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -299,7 +303,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -334,7 +338,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -511,7 +515,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -521,25 +525,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="59.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="53.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.7109375" customWidth="1"/>
     <col min="11" max="11" width="25.5703125" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.5703125" customWidth="1"/>
+    <col min="13" max="13" width="24.28515625" customWidth="1"/>
     <col min="14" max="14" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.42578125" customWidth="1"/>
     <col min="16" max="16" width="25.7109375" bestFit="1" customWidth="1"/>
@@ -548,261 +552,261 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="E2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" s="9" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="3" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="12" t="s">
+      <c r="P3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="R3" s="15" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="9">
+        <v>60.55</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="7">
+        <v>1234561</v>
+      </c>
+      <c r="I4" s="8">
+        <v>42019</v>
+      </c>
+      <c r="J4" s="8">
+        <v>43546</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="7">
+        <v>123456</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="15">
-        <v>60.55</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="13">
-        <v>1234561</v>
-      </c>
-      <c r="I4" s="14">
-        <v>42019</v>
-      </c>
-      <c r="J4" s="14">
-        <v>43546</v>
-      </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="13">
-        <v>123456</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="P4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q4" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="R4" s="13"/>
+      <c r="Q4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="7"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="A5" s="7">
         <v>2</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="9">
+        <v>3.8</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="7">
+        <v>1234561</v>
+      </c>
+      <c r="I5" s="8">
+        <v>42019</v>
+      </c>
+      <c r="J5" s="8">
+        <v>43546</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="7">
+        <v>123456</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="15">
-        <v>3.8</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="13">
-        <v>1234561</v>
-      </c>
-      <c r="I5" s="14">
-        <v>42019</v>
-      </c>
-      <c r="J5" s="14">
-        <v>43546</v>
-      </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" s="13">
-        <v>123456</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="P5" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q5" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="R5" s="13"/>
+      <c r="Q5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" s="7"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="9">
+        <v>50</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="7">
+        <v>1234572</v>
+      </c>
+      <c r="I6" s="8">
+        <v>42141</v>
+      </c>
+      <c r="J6" s="8">
+        <v>43546</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="7">
+        <v>123457</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="15">
-        <v>50</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="13">
-        <v>1234572</v>
-      </c>
-      <c r="I6" s="14">
-        <v>42141</v>
-      </c>
-      <c r="J6" s="14">
-        <v>43546</v>
-      </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" s="13">
-        <v>123457</v>
-      </c>
-      <c r="O6" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="P6" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q6" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="R6" s="13"/>
+      <c r="R6" s="7"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
+      <c r="A7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#SSW-1763 Import Fakturierung überarbeitung + jährliche Zahlung, +refactor
</commit_message>
<xml_diff>
--- a/Common/Style/Resource/Template/Fakturierung Import.xlsx
+++ b/Common/Style/Resource/Template/Fakturierung Import.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rackel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siddy\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F45428-4A64-4088-8A01-AECF078EB975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730"/>
+    <workbookView xWindow="1875" yWindow="4890" windowWidth="23865" windowHeight="15630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$3:$R$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$3:$S$10</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
   <si>
     <t>Beitragsart</t>
   </si>
@@ -63,9 +64,6 @@
     <t>Datum beitragspflichtig von</t>
   </si>
   <si>
-    <t>Datum beitragspflichtig bis</t>
-  </si>
-  <si>
     <t>*Ab wann soll die Zahlung gelten (aktuelles Datum)</t>
   </si>
   <si>
@@ -79,9 +77,6 @@
   </si>
   <si>
     <t>Kontoinhaber</t>
-  </si>
-  <si>
-    <t>*Ab wann soll die Zahlung nicht mehr gezogen werden</t>
   </si>
   <si>
     <t>Bitte lassen Sie die ersten 3 Zeilen unangetastet, 
@@ -160,12 +155,27 @@
   </si>
   <si>
     <t>Beitragszahler Nachname</t>
+  </si>
+  <si>
+    <t>* mit X markieren, wenn zutreffend</t>
+  </si>
+  <si>
+    <t>Zahlung Jährlich</t>
+  </si>
+  <si>
+    <t>Beispieldaten danach sollten überschrieben werden</t>
+  </si>
+  <si>
+    <t>*Ab wann soll die Zahlung nicht mehr gezogen werden</t>
+  </si>
+  <si>
+    <t>Datum beitragspflichtig bis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ _€"/>
   </numFmts>
@@ -216,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -242,6 +252,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -522,11 +540,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,28 +556,33 @@
     <col min="5" max="5" width="41.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="30.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" customWidth="1"/>
-    <col min="11" max="11" width="25.5703125" customWidth="1"/>
-    <col min="12" max="12" width="22.5703125" customWidth="1"/>
-    <col min="13" max="13" width="24.28515625" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" customWidth="1"/>
-    <col min="16" max="16" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="12" max="12" width="26.42578125" customWidth="1"/>
+    <col min="13" max="13" width="22.5703125" customWidth="1"/>
+    <col min="14" max="14" width="24.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.42578125" customWidth="1"/>
+    <col min="17" max="17" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" customWidth="1"/>
+    <col min="19" max="19" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="17"/>
     </row>
-    <row r="2" spans="1:18" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -567,118 +590,121 @@
         <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="C3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="5" t="s">
+      <c r="D3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>19</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="11" t="s">
+      <c r="O3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="10" t="s">
-        <v>16</v>
-      </c>
       <c r="P3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="R3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="15" t="s">
-        <v>15</v>
+      <c r="S3" s="15" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="9">
         <v>60.55</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="7">
+      <c r="I4" s="7">
         <v>1234561</v>
       </c>
-      <c r="I4" s="8">
+      <c r="J4" s="8">
         <v>42019</v>
       </c>
-      <c r="J4" s="8">
+      <c r="K4" s="8">
         <v>43546</v>
       </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="L4" s="17"/>
       <c r="M4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" s="7">
         <v>123456</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="P4" s="7" t="s">
         <v>31</v>
@@ -686,17 +712,20 @@
       <c r="Q4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="7"/>
+      <c r="R4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="9">
@@ -706,27 +735,24 @@
       <c r="G5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="7">
+      <c r="I5" s="7">
         <v>1234561</v>
       </c>
-      <c r="I5" s="8">
+      <c r="J5" s="8">
         <v>42019</v>
       </c>
-      <c r="J5" s="8">
+      <c r="K5" s="8">
         <v>43546</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="L5" s="17"/>
       <c r="M5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="7">
         <v>123456</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="P5" s="7" t="s">
         <v>31</v>
@@ -734,49 +760,49 @@
       <c r="Q5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R5" s="7"/>
+      <c r="R5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="9">
         <v>50</v>
       </c>
       <c r="F6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="7">
+        <v>1234572</v>
+      </c>
+      <c r="J6" s="8">
+        <v>42141</v>
+      </c>
+      <c r="K6" s="8">
+        <v>43546</v>
+      </c>
+      <c r="L6" s="17"/>
+      <c r="M6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="7">
-        <v>1234572</v>
-      </c>
-      <c r="I6" s="8">
-        <v>42141</v>
-      </c>
-      <c r="J6" s="8">
-        <v>43546</v>
-      </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N6" s="7">
+      <c r="N6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="7">
         <v>123457</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="P6" s="7" t="s">
         <v>32</v>
@@ -784,11 +810,14 @@
       <c r="Q6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="R6" s="7"/>
+      <c r="R6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -796,17 +825,17 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
+      <c r="L7" s="17"/>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>